<commit_message>
update 30 maret 2024 dan ioncube
</commit_message>
<xml_diff>
--- a/assets/template/template_guru.xlsx
+++ b/assets/template/template_guru.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>No</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -439,11 +442,11 @@
     <col min="5" max="5" width="22.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" hidden="1"/>
+    <col min="8" max="9" width="24.28515625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -468,8 +471,11 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -494,8 +500,9 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -504,8 +511,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -514,8 +522,9 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -524,8 +533,9 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -534,8 +544,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -544,8 +555,9 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -554,8 +566,9 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -564,8 +577,9 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -574,8 +588,9 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -584,8 +599,9 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -594,8 +610,9 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -604,8 +621,9 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -614,8 +632,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -624,8 +643,9 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -634,8 +654,9 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -644,8 +665,9 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -654,8 +676,9 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -664,8 +687,9 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -674,8 +698,9 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -684,8 +709,9 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -694,8 +720,9 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -704,8 +731,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -714,8 +742,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -724,8 +753,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -734,8 +764,9 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -744,8 +775,9 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -754,8 +786,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -764,8 +797,9 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -774,8 +808,9 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -784,8 +819,9 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -794,8 +830,9 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -804,8 +841,9 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -814,8 +852,9 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -824,8 +863,9 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -834,8 +874,9 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -844,8 +885,9 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -854,8 +896,9 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -864,8 +907,9 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -874,8 +918,9 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -884,8 +929,9 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -894,8 +940,9 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -904,8 +951,9 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -914,8 +962,9 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -924,8 +973,9 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -934,8 +984,9 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -944,8 +995,9 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -954,8 +1006,9 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -964,8 +1017,9 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -974,8 +1028,9 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -984,8 +1039,9 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -994,8 +1050,9 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1004,8 +1061,9 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1014,8 +1072,9 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1024,8 +1083,9 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1034,8 +1094,9 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1044,8 +1105,9 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1054,8 +1116,9 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1064,8 +1127,9 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1074,8 +1138,9 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1084,8 +1149,9 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1094,8 +1160,9 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1104,8 +1171,9 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1114,8 +1182,9 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1124,8 +1193,9 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1134,8 +1204,9 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1144,8 +1215,9 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1154,8 +1226,9 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1164,8 +1237,9 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1174,8 +1248,9 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1184,8 +1259,9 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1194,8 +1270,9 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1204,8 +1281,9 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1214,8 +1292,9 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1224,8 +1303,9 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1234,8 +1314,9 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1244,8 +1325,9 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1254,8 +1336,9 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1264,8 +1347,9 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1274,8 +1358,9 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1284,8 +1369,9 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1294,8 +1380,9 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1304,8 +1391,9 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1314,8 +1402,9 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1324,8 +1413,9 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1334,8 +1424,9 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1344,8 +1435,9 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1354,8 +1446,9 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1364,8 +1457,9 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1374,8 +1468,9 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1384,8 +1479,9 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1394,8 +1490,9 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1404,8 +1501,9 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1414,8 +1512,9 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1424,8 +1523,9 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1434,8 +1534,9 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1444,8 +1545,9 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1454,8 +1556,9 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1464,8 +1567,9 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1474,8 +1578,9 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1484,6 +1589,7 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>